<commit_message>
In Doc Vals I bring the Captivate throughout the script and some new changes in the script
</commit_message>
<xml_diff>
--- a/XLSX/Operational PortalDataForm.xlsx
+++ b/XLSX/Operational PortalDataForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradeep\Marquis\Master download\23-02-2023\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Marquis\Daily Automation\from MAster\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BFBDFC-61F2-4C35-B2FD-2BE8EFB209E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D742534-B378-438A-A8E9-085AD8F671A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11112" xr2:uid="{6D2CF105-7DB3-4735-9888-FFF71A4D6BC7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6D2CF105-7DB3-4735-9888-FFF71A4D6BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="DocVals" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>Checklist Table</t>
   </si>
@@ -72,163 +83,160 @@
     <t>Pass/Fail/NA</t>
   </si>
   <si>
+    <t>Validation Status Table</t>
+  </si>
+  <si>
+    <t>30- Day Pay Out Check</t>
+  </si>
+  <si>
+    <t>KYC Outcome</t>
+  </si>
+  <si>
+    <t>AVS Outcome</t>
+  </si>
+  <si>
+    <t>POI Outcome</t>
+  </si>
+  <si>
+    <t>Check Options</t>
+  </si>
+  <si>
+    <t>Approve/Reject/Retry</t>
+  </si>
+  <si>
+    <t>POR/KYC Outcome Table</t>
+  </si>
+  <si>
+    <t>POR Outcome</t>
+  </si>
+  <si>
+    <t>KYC Fraud Outcome</t>
+  </si>
+  <si>
+    <t>AML Outcome</t>
+  </si>
+  <si>
+    <t>Retry</t>
+  </si>
+  <si>
+    <t>Final Approvals</t>
+  </si>
+  <si>
+    <t>Approve Vals</t>
+  </si>
+  <si>
+    <t>Reject Vals</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>POI Outcome- Reject Reasons.</t>
+  </si>
+  <si>
+    <t>Submit 3 months’ BS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Submit 3 additional months’ BS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Submit payslip</t>
+  </si>
+  <si>
+    <t>Submit ITA34</t>
+  </si>
+  <si>
+    <t>Submit pension letter</t>
+  </si>
+  <si>
+    <t>Submit increase letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Submit latest CIPC cert.</t>
+  </si>
+  <si>
+    <t>Submit latest audited FinStat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amend income details &amp;resubmit</t>
+  </si>
+  <si>
+    <t>Resubmit ID Copy</t>
+  </si>
+  <si>
+    <t>Amend cust name per ID doc</t>
+  </si>
+  <si>
+    <t>Resubmit back/front of ID Card</t>
+  </si>
+  <si>
+    <t>Submit marriage certificate</t>
+  </si>
+  <si>
+    <t>Submit affidavit - tempID/PPT</t>
+  </si>
+  <si>
+    <t>BankDetails must belong toCust</t>
+  </si>
+  <si>
+    <t>Amend banking details</t>
+  </si>
+  <si>
+    <t>Submit POA declarationEvidence</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>KYC - Outcome -Rejection Reasons</t>
+  </si>
+  <si>
+    <t>AVS Outcome Rejection-Reasons</t>
+  </si>
+  <si>
+    <t>POR Outcome- Rejection Reasons</t>
+  </si>
+  <si>
+    <t>KYC Fraud Outcome - Rejection Reasons</t>
+  </si>
+  <si>
+    <t>Operational User</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Bhairub</t>
+  </si>
+  <si>
+    <t>WFG6eKRvi3kvpQ</t>
+  </si>
+  <si>
+    <t>Resubmit ID Copy-k</t>
+  </si>
+  <si>
+    <t>Amend cust name per ID doc-k</t>
+  </si>
+  <si>
+    <t>Resubmit back/front of ID Card-k</t>
+  </si>
+  <si>
+    <t>Submit marriage certificate-k</t>
+  </si>
+  <si>
+    <t>Submit affidavit - tempID/PPT-k</t>
+  </si>
+  <si>
+    <t>Submit valid proof of address</t>
+  </si>
+  <si>
     <t>pass</t>
   </si>
   <si>
-    <t>Validation Status Table</t>
-  </si>
-  <si>
-    <t>30- Day Pay Out Check</t>
-  </si>
-  <si>
-    <t>KYC Outcome</t>
-  </si>
-  <si>
-    <t>AVS Outcome</t>
-  </si>
-  <si>
-    <t>POI Outcome</t>
-  </si>
-  <si>
-    <t>Check Options</t>
-  </si>
-  <si>
-    <t>Approve/Reject/Retry</t>
-  </si>
-  <si>
-    <t>POR/KYC Outcome Table</t>
-  </si>
-  <si>
-    <t>POR Outcome</t>
-  </si>
-  <si>
-    <t>KYC Fraud Outcome</t>
-  </si>
-  <si>
-    <t>AML Outcome</t>
-  </si>
-  <si>
-    <t>Retry</t>
-  </si>
-  <si>
-    <t>Final Approvals</t>
-  </si>
-  <si>
-    <t>Approve Vals</t>
-  </si>
-  <si>
-    <t>Reject Vals</t>
-  </si>
-  <si>
-    <t>Click</t>
-  </si>
-  <si>
-    <t>POI Outcome- Reject Reasons.</t>
-  </si>
-  <si>
-    <t>Submit 3 months’ BS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Submit 3 additional months’ BS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Submit payslip</t>
-  </si>
-  <si>
-    <t>Submit ITA34</t>
-  </si>
-  <si>
-    <t>Submit pension letter</t>
-  </si>
-  <si>
-    <t>Submit increase letter</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Submit latest CIPC cert.</t>
-  </si>
-  <si>
-    <t>Submit latest audited FinStat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amend income details &amp;resubmit</t>
-  </si>
-  <si>
-    <t>Resubmit ID Copy</t>
-  </si>
-  <si>
-    <t>Amend cust name per ID doc</t>
-  </si>
-  <si>
-    <t>Resubmit back/front of ID Card</t>
-  </si>
-  <si>
-    <t>Submit marriage certificate</t>
-  </si>
-  <si>
-    <t>Submit affidavit - tempID/PPT</t>
-  </si>
-  <si>
-    <t>BankDetails must belong toCust</t>
-  </si>
-  <si>
-    <t>Amend banking details</t>
-  </si>
-  <si>
-    <t>Submit POA declarationEvidence</t>
-  </si>
-  <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>KYC - Outcome -Rejection Reasons</t>
-  </si>
-  <si>
-    <t>AVS Outcome Rejection-Reasons</t>
-  </si>
-  <si>
-    <t>POR Outcome- Rejection Reasons</t>
-  </si>
-  <si>
-    <t>KYC Fraud Outcome - Rejection Reasons</t>
-  </si>
-  <si>
-    <t>Operational User</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Approve</t>
-  </si>
-  <si>
-    <t>Resubmit ID Copy-k</t>
-  </si>
-  <si>
-    <t>Amend cust name per ID doc-k</t>
-  </si>
-  <si>
-    <t>Resubmit back/front of ID Card-k</t>
-  </si>
-  <si>
-    <t>Submit marriage certificate-k</t>
-  </si>
-  <si>
-    <t>Submit affidavit - tempID/PPT-k</t>
-  </si>
-  <si>
-    <t>Submit valid proof of address</t>
-  </si>
-  <si>
-    <t>Fer1C623RGRvD4mN%C</t>
-  </si>
-  <si>
-    <t>raghup</t>
   </si>
 </sst>
 </file>
@@ -735,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341C3EC0-A8D8-42A3-B485-490C2BB3164F}">
   <dimension ref="A1:CM15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BK5" sqref="BK5"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BN3" sqref="BN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,7 +800,7 @@
       <c r="M1" s="26"/>
       <c r="N1" s="21"/>
       <c r="O1" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P1" s="26"/>
       <c r="Q1" s="26"/>
@@ -800,19 +808,19 @@
       <c r="S1" s="26"/>
       <c r="T1" s="21"/>
       <c r="U1" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V1" s="26"/>
       <c r="W1" s="26"/>
       <c r="X1" s="26"/>
       <c r="Y1" s="21"/>
       <c r="Z1" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA1" s="24"/>
       <c r="AB1" s="21"/>
       <c r="AC1" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
@@ -825,7 +833,7 @@
       <c r="AL1" s="27"/>
       <c r="AM1" s="21"/>
       <c r="AN1" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AO1" s="22"/>
       <c r="AP1" s="22"/>
@@ -834,19 +842,19 @@
       <c r="AS1" s="22"/>
       <c r="AT1" s="21"/>
       <c r="AU1" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AV1" s="22"/>
       <c r="AW1" s="22"/>
       <c r="AX1" s="21"/>
       <c r="AY1" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AZ1" s="22"/>
       <c r="BA1" s="22"/>
       <c r="BB1" s="21"/>
       <c r="BC1" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="22"/>
       <c r="BE1" s="22"/>
@@ -855,7 +863,7 @@
       <c r="BH1" s="22"/>
       <c r="BI1" s="21"/>
       <c r="BJ1" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BK1" s="22"/>
     </row>
@@ -901,135 +909,135 @@
       </c>
       <c r="N2" s="21"/>
       <c r="O2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="T2" s="21"/>
       <c r="U2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="Y2" s="21"/>
       <c r="Z2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="AB2" s="21"/>
       <c r="AC2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AD2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="AM2" s="21"/>
       <c r="AN2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AO2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="AT2" s="21"/>
       <c r="AU2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AV2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="AX2" s="21"/>
       <c r="AY2" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BB2" s="21"/>
       <c r="BC2" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="BD2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BE2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="BH2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="BI2" s="21"/>
       <c r="BJ2" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="BK2" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="BK2" s="20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:91" ht="36" x14ac:dyDescent="0.3">
@@ -1037,160 +1045,160 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="N3" s="21"/>
       <c r="O3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="T3" s="21"/>
       <c r="U3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y3" s="21"/>
       <c r="Z3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="21"/>
       <c r="AC3" s="23"/>
       <c r="AD3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AJ3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AM3" s="21"/>
       <c r="AN3" s="23"/>
       <c r="AO3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AP3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AQ3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AR3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AS3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AT3" s="21"/>
       <c r="AU3" s="23"/>
       <c r="AV3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AW3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AX3" s="21"/>
       <c r="AY3" s="25"/>
       <c r="AZ3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BA3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BB3" s="21"/>
       <c r="BC3" s="25"/>
       <c r="BD3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BE3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BF3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BG3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BH3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BI3" s="21"/>
       <c r="BJ3" s="5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="BK3" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:91" x14ac:dyDescent="0.3">

</xml_diff>